<commit_message>
Updated the batch & excel
</commit_message>
<xml_diff>
--- a/jcp-v2/04-rsconnectProfiles/LOT_Div1-20Feb_v2_VSmall.xlsx
+++ b/jcp-v2/04-rsconnectProfiles/LOT_Div1-20Feb_v2_VSmall.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="3540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
+    <t>Id</t>
+  </si>
+  <si>
     <t>Creation Date</t>
   </si>
   <si>
+    <t>On-Site Date</t>
+  </si>
+  <si>
+    <t>Off-Site Date</t>
+  </si>
+  <si>
     <t>Display Name</t>
   </si>
   <si>
@@ -38,6 +47,9 @@
     <t>Online Only</t>
   </si>
   <si>
+    <t>Short Name</t>
+  </si>
+  <si>
     <t>1071108</t>
   </si>
   <si>
@@ -90,18 +102,6 @@
   </si>
   <si>
     <t>BLK/WHT SHORT BRIM DRESSY HAT</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>On-Site Date</t>
-  </si>
-  <si>
-    <t>Off-Site Date</t>
-  </si>
-  <si>
-    <t>Short Name</t>
   </si>
 </sst>
 </file>
@@ -420,62 +420,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -483,22 +479,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -506,22 +502,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -529,41 +525,23 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>